<commit_message>
added validation expression to sheet
</commit_message>
<xml_diff>
--- a/molgenis-platform-integration-tests/src/test/resources/xls/it_emx_nullable_expressions.xlsx
+++ b/molgenis-platform-integration-tests/src/test/resources/xls/it_emx_nullable_expressions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/IdeaProjects/molgenis/molgenis-platform-integration-tests/src/test/resources/xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A5263B7E-DFCD-E442-8801-1FE201BB1D74}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1CE1F002-8E96-D44B-8B5C-66B6C7DED55C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="880" firstSheet="3" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="241">
   <si>
     <t>name</t>
   </si>
@@ -754,6 +754,12 @@
   </si>
   <si>
     <t>$("name").value() === 'MOLGENIS'</t>
+  </si>
+  <si>
+    <t>validationExpression</t>
+  </si>
+  <si>
+    <t>$("name").value() !== 'not valid'</t>
   </si>
 </sst>
 </file>
@@ -1825,10 +1831,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1847,10 +1853,11 @@
     <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="81.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="1025" width="8.83203125" customWidth="1"/>
+    <col min="15" max="15" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1896,8 +1903,11 @@
       <c r="O1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1926,7 +1936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -1940,7 +1950,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -1957,7 +1967,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1979,8 +1989,11 @@
       <c r="O5" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -2000,7 +2013,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>209</v>
       </c>
@@ -2023,7 +2036,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>214</v>
       </c>
@@ -2049,7 +2062,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>211</v>
       </c>
@@ -2072,7 +2085,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -2089,7 +2102,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -2112,7 +2125,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -2138,7 +2151,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>224</v>
       </c>
@@ -2155,7 +2168,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -2178,7 +2191,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>163</v>
       </c>
@@ -2204,7 +2217,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>162</v>
       </c>

</xml_diff>